<commit_message>
Computing MAPE errors, "shift" dummy
</commit_message>
<xml_diff>
--- a/sarimaresults.xlsx
+++ b/sarimaresults.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_4F7AFDCE8F79A8536E3CA493EAB4E2B379B6C787" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B3D686B-AC3C-4712-8F6A-4C1010766BCA}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_4F7AFDCE8F79A8536E3CA493EAB4E2B379B6C787" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34083A9A-864A-4FD2-B6DC-1775C466C027}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>h1</t>
   </si>
@@ -64,15 +65,51 @@
   <si>
     <t>SARIMA</t>
   </si>
+  <si>
+    <t>&gt; dm_tests[["pvalues"]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              1              4             </t>
+  </si>
+  <si>
+    <t>LASSO         "0.2163739993" "0.0960763961"</t>
+  </si>
+  <si>
+    <t>Elastic Net   "0.1784399960" "0.1017372032"</t>
+  </si>
+  <si>
+    <t>Random Forest "0.2446652745" "0.0680660232"</t>
+  </si>
+  <si>
+    <t>&gt; dm_test_mean = compute_dmv2()</t>
+  </si>
+  <si>
+    <t>&gt; View(dm_test_mean)</t>
+  </si>
+  <si>
+    <t>&gt; dm_test_mean[["pvalues"]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              1                4              </t>
+  </si>
+  <si>
+    <t>LASSO         "0.0229841679*"  "0.0344298305*"</t>
+  </si>
+  <si>
+    <t>Elastic Net   "0.0058906825**" "0.0121609194*"</t>
+  </si>
+  <si>
+    <t>Random Forest "0.0083655265**" "0.0241920941*"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,13 +125,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF4D4D4C"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF8959A8"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,7 +173,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1575,15 +1642,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>215899</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1609,6 +1676,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1900,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3026,8 +3097,8 @@
         <v>7.9801105108028875E-2</v>
       </c>
       <c r="L31" s="4">
-        <f>AVERAGE(L2:L29)*100</f>
-        <v>99.584755703316901</v>
+        <f>MEDIAN(L2:L29)*100</f>
+        <v>56.551224071629093</v>
       </c>
       <c r="M31" s="4">
         <f>AVERAGE(M2:M29)*100</f>
@@ -3038,4 +3109,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE36F37-4973-412E-AFDA-5BDA03B7539A}">
+  <dimension ref="B3:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>